<commit_message>
Graphics for Small Instances (10, 15 and 20 jobs)
</commit_message>
<xml_diff>
--- a/General Results/Average RPD Data Large Instances.xlsx
+++ b/General Results/Average RPD Data Large Instances.xlsx
@@ -599,99 +599,99 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="43" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="37" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="45" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="36" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="39" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="40" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="43" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="42" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="39" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="45" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="36" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
@@ -699,27 +699,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="38" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
@@ -727,31 +727,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="35" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="41" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="38" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="35" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable45.xml><?xml version="1.0" encoding="utf-8"?>
@@ -759,23 +759,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="3_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="40" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_50jobs" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="4_FINAL_ILS_PROP_OBJ_F_80jobs" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="5_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="37" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1_FINAL_ILS_PROP_OBJ_F_100jobs" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1067,7 +1067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P541"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A529" workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
@@ -22722,7 +22722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M541"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A394" workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
@@ -66019,10 +66019,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G542"/>
+  <dimension ref="A1:J542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A517" workbookViewId="0">
-      <selection activeCell="C361" sqref="C361:E542"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66034,7 +66034,7 @@
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
@@ -66043,7 +66043,7 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -66057,7 +66057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>MIN(ILS_RVND_1!L2, ILS_RVND_2!L2, AG_LS!L2)</f>
         <v>272628.59999999998</v>
@@ -66075,7 +66075,7 @@
         <v>0.47705926670937499</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>MIN(ILS_RVND_1!L3, ILS_RVND_2!L3, AG_LS!L3)</f>
         <v>277153.40000000002</v>
@@ -66092,8 +66092,9 @@
         <f>100 * ((AG_LS!L3-A4)/A4)</f>
         <v>0.92418133784393941</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>MIN(ILS_RVND_1!L4, ILS_RVND_2!L4, AG_LS!L4)</f>
         <v>274257.40000000002</v>
@@ -66111,7 +66112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>MIN(ILS_RVND_1!L5, ILS_RVND_2!L5, AG_LS!L5)</f>
         <v>268834.8</v>
@@ -66129,7 +66130,7 @@
         <v>2.5152993585651857</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>MIN(ILS_RVND_1!L6, ILS_RVND_2!L6, AG_LS!L6)</f>
         <v>259685.6</v>
@@ -66147,7 +66148,7 @@
         <v>1.0378704094489577</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>MIN(ILS_RVND_1!L7, ILS_RVND_2!L7, AG_LS!L7)</f>
         <v>270296.59999999998</v>
@@ -66165,7 +66166,7 @@
         <v>0.52816054659956324</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>MIN(ILS_RVND_1!L8, ILS_RVND_2!L8, AG_LS!L8)</f>
         <v>236799.6</v>
@@ -66183,7 +66184,7 @@
         <v>2.527538053273731</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>MIN(ILS_RVND_1!L9, ILS_RVND_2!L9, AG_LS!L9)</f>
         <v>309597</v>
@@ -66201,7 +66202,7 @@
         <v>1.8750827688898832</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>MIN(ILS_RVND_1!L10, ILS_RVND_2!L10, AG_LS!L10)</f>
         <v>251417</v>
@@ -66219,7 +66220,7 @@
         <v>0.75539840185827201</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>MIN(ILS_RVND_1!L11, ILS_RVND_2!L11, AG_LS!L11)</f>
         <v>293640.40000000002</v>
@@ -66237,7 +66238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>MIN(ILS_RVND_1!L12, ILS_RVND_2!L12, AG_LS!L12)</f>
         <v>284967.8</v>
@@ -66255,7 +66256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>MIN(ILS_RVND_1!L13, ILS_RVND_2!L13, AG_LS!L13)</f>
         <v>264097.40000000002</v>
@@ -66273,7 +66274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>MIN(ILS_RVND_1!L14, ILS_RVND_2!L14, AG_LS!L14)</f>
         <v>254360</v>
@@ -66291,7 +66292,7 @@
         <v>0.97365938040572653</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>MIN(ILS_RVND_1!L15, ILS_RVND_2!L15, AG_LS!L15)</f>
         <v>312768.8</v>
@@ -75783,5 +75784,6 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>